<commit_message>
Styling, changed logo, modified system prompt for saying no for answers it does not know. Added error handling
</commit_message>
<xml_diff>
--- a/data_v2.xlsx
+++ b/data_v2.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev02chandan/Documents/Intern@MatiriAI/Property LLM/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F9C039-85F1-FB4A-BC94-A77AADF70304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -490,6 +484,40 @@
     <t>The home can accommodate up to 10 guests across 3 bedrooms, futon, and a 2 queen sofa sleeper in the living room. Each bedroom features a king-size bed. Two of the bedrooms have private ensuite bathrooms, while the third offers a Jack and Jill style bathroom.</t>
   </si>
   <si>
+    <t xml:space="preserve">Property Name: The Real McCoy
+Address: 2424 Walnut Ridge Way, Sevierville, TN 37862, US
+Description: 1 set of towels (bath towel, hand towel, washcloth) per occupant (up to max occupancy on listing)
+ 2 rolls of toilet paper, bar soap or liquid soap dispenser, and wastebasket trash bag per bathroom
+ Shampoo, Conditioner, &amp; Body Wash pump bottle per full bathroom
+ 2 rolls of paper towels, fresh sponge, dish soap, 3 loads of dishwasher detergent, 3 trash bags per kitchen.
+ 3 loads of laundry detergent per home (with in-house laundry systems)
+Max Occupancy: 10
+Bedrooms: 3, Full Bathrooms: 3, Three Quarter Bathrooms: 0, Half Bathrooms: 0
+Check-in Time: 16:00:00, Check-out Time: 10:00:00, Early Check-in Time: 12:00:00, Late Check-out Time: 15:00:00
+Access: There is parking space provided for 2-3 vehicles in the private paved roundabout driveway directly in front of the property. 
+ The entry door is equipped with an electronic lock
+ The code will activate right at 4 PM
+ To unlock, enter the code provided, the lock will flash green, then turn the deadbolt.
+ The door does NOT lock automatically so please lock it when you leave.
+ To lock, turn the deadbolt.
+ Wifi Name
+ The Real McCoy
+ Wifi Password
+ 8657747966
+ Wifi Notes
+ Wifi Router Location
+ Lower Level | Game Room | In the cabinet behind TV
+Location: The Real McCoy, a hidden retreat, is located in the rural part of Sevierville, Tennessee. This authentic downtown area is famous for its shopping options and proximity to the Great Smoky Mountains National Park. The home offers a unique off-the-beaten-path experience designed for those who seek stunning views, custom carpentry, and thoughtfully curated amenities.
+Outdoor Features: The property features extensive deck space, where you can soak in breathtaking views. Enjoy the tranquility and rich landscape from the comfort of the rocking chairs, making it a perfect spot for a serene morning coffee or reading session.
+Interior Amenities: Inside, the home presents a unique blend of a traditional cabin and a treehouse. The floor-to-ceiling wooden planks and large windows overlooking the treetops create a warm, organic ambiance. The living room boasts high peaked ceilings, ample seating, and deck access. A smart TV and a fireplace further enhance the cozy, relaxing environment. The kitchen is well-equipped with stainless steel appliances, including a blender, toaster, and coffee maker for your convenience. Mealtime options include a dining table inside or an al fresco setting on the deck.
+Sleeping Arrangements: The home can accommodate up to 10 guests across 3 bedrooms, futon, and a 2 queen sofa sleeper in the living room. Each bedroom features a king-size bed. Two of the bedrooms have private ensuite bathrooms, while the third offers a Jack and Jill style bathroom.
+Latitude: 35.75112, Longitude: -83.6085
+Property Website on Grand Welcome: https://www.grandwelcome.com/vrp/unit/The_Real_McCoy-102369-15
+Property Website on Airbnb: https://www.airbnb.com/rooms/658522003554413078
+Contacts:  Property Manager: 123456789 , FireFly Lawn Care:   +1 865-607-7520
+</t>
+  </si>
+  <si>
     <t xml:space="preserve"> (FireFly Lawn Care   +1 865-607-7520)</t>
   </si>
   <si>
@@ -703,7 +731,7 @@
 Latitude: 35.71308, Longitude: -83.6179
 Property Listing on Grand Welcome: https://www.grandwelcome.com/vrp/unit/Treetop_Paradise-102402-15
 Property Listing on Airbnb: https://www.airbnb.com/rooms/669464604242003293
-Contacts:  Property Manager:+1 865-453-5861, Arrow Exterminators:+1 865-453-5860,   FireFly Lawn Care: +1 865-607-7520
+Contacts:  Property Manager: 1234567890, Arrow Exterminators:+1 865-453-5860,   FireFly Lawn Care: +1 865-607-7520
 </t>
   </si>
   <si>
@@ -924,7 +952,7 @@
 Latitude: 35.79348, Longitude: -83.4143
 Property Listing on Grand Welcome: https://www.grandwelcome.com/vrp/unit/Rays_Chalet-102536-15
 Property Listing on Airbnb: https://www.airbnb.com/rooms/725931619348454163
-Contacts:  Property Manager: +1 865-453-5860, JerryCindy   +1 865-654-9031
+Contacts:  Property Manager: 1234567890, JerryCindy   +1 865-654-9031
 </t>
   </si>
   <si>
@@ -1159,7 +1187,7 @@
 Latitude: 35.77981, Longitude: -83.6633
 Property Listing on Grand Welcome: https://www.grandwelcome.com/vrp/unit/Bearfoot_Landing-102706-15
 Property Listing on Airbnb: https://www.airbnb.com/rooms/766599293166468020
-Contacts:  Property Manager: +1 865-453-5860, Arrow Exterminators: +1 865-206-9489, FireFly Lawn Care: +1 865-607-7520, Ridge Valley Heat: +1 865-428-6491
+Contacts:  Property Manager: 1234567890, Arrow Exterminators: +1 865-206-9489, FireFly Lawn Care: +1 865-607-7520, Ridge Valley Heat: +1 865-428-6491
 </t>
   </si>
   <si>
@@ -1376,7 +1404,7 @@
 Latitude: 35.81405, Longitude: -83.608
 Property Listing on Grand Welcome: https://www.grandwelcome.com/vrp/unit/Sliver_of_Paradise-102756-15
 Property Listing on Airbnb: https://www.airbnb.com/rooms/785464657702765446
-Contacts:  Property Manager: +1 865-453-5860, Arrow Exterminators   +1 865-453-5860
+Contacts:  Property Manager: 1234567890, Arrow Exterminators   +1 865-453-5860
 </t>
   </si>
   <si>
@@ -2187,48 +2215,15 @@
 Latitude: 35.8101, Longitude: -83.5227
 Property Listing on Grand Welcome: https://www.grandwelcome.com/vrp/unit/Woodland_Wonder-102853-15
 Property Listing on Airbnb: https://www.airbnb.com/rooms/815888950061579742
-Contacts:  (Arrow Exterminators   +1 865-453-5860   FireFly Lawn Care   +1 865-607-7520)
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Property Name: The Real McCoy
-Address: 2424 Walnut Ridge Way, Sevierville, TN 37862, US
-Description: 1 set of towels (bath towel, hand towel, washcloth) per occupant (up to max occupancy on listing)
- 2 rolls of toilet paper, bar soap or liquid soap dispenser, and wastebasket trash bag per bathroom
- Shampoo, Conditioner, &amp; Body Wash pump bottle per full bathroom
- 2 rolls of paper towels, fresh sponge, dish soap, 3 loads of dishwasher detergent, 3 trash bags per kitchen.
- 3 loads of laundry detergent per home (with in-house laundry systems)
-Max Occupancy: 10
-Bedrooms: 3, Full Bathrooms: 3, Three Quarter Bathrooms: 0, Half Bathrooms: 0
-Check-in Time: 16:00:00, Check-out Time: 10:00:00, Early Check-in Time: 12:00:00, Late Check-out Time: 15:00:00
-Access: There is parking space provided for 2-3 vehicles in the private paved roundabout driveway directly in front of the property. 
- The entry door is equipped with an electronic lock
- The code will activate right at 4 PM
- To unlock, enter the code provided, the lock will flash green, then turn the deadbolt.
- The door does NOT lock automatically so please lock it when you leave.
- To lock, turn the deadbolt.
- Wifi Name
- The Real McCoy
- Wifi Password
- 8657747966
- Wifi Notes
- Wifi Router Location
- Lower Level | Game Room | In the cabinet behind TV
-Location: The Real McCoy, a hidden retreat, is located in the rural part of Sevierville, Tennessee. This authentic downtown area is famous for its shopping options and proximity to the Great Smoky Mountains National Park. The home offers a unique off-the-beaten-path experience designed for those who seek stunning views, custom carpentry, and thoughtfully curated amenities.
-Outdoor Features: The property features extensive deck space, where you can soak in breathtaking views. Enjoy the tranquility and rich landscape from the comfort of the rocking chairs, making it a perfect spot for a serene morning coffee or reading session.
-Interior Amenities: Inside, the home presents a unique blend of a traditional cabin and a treehouse. The floor-to-ceiling wooden planks and large windows overlooking the treetops create a warm, organic ambiance. The living room boasts high peaked ceilings, ample seating, and deck access. A smart TV and a fireplace further enhance the cozy, relaxing environment. The kitchen is well-equipped with stainless steel appliances, including a blender, toaster, and coffee maker for your convenience. Mealtime options include a dining table inside or an al fresco setting on the deck.
-Sleeping Arrangements: The home can accommodate up to 10 guests across 3 bedrooms, futon, and a 2 queen sofa sleeper in the living room. Each bedroom features a king-size bed. Two of the bedrooms have private ensuite bathrooms, while the third offers a Jack and Jill style bathroom.
-Latitude: 35.75112, Longitude: -83.6085
-Property Website on Grand Welcome: https://www.grandwelcome.com/vrp/unit/The_Real_McCoy-102369-15
-Property Website on Airbnb: https://www.airbnb.com/rooms/658522003554413078
-Contacts:  Property Manager: +1 865-608-7432 , FireFly Lawn Care:   +1 865-607-7520
+Contacts:  Arrow Exterminators: +1 865-453-5860, FireFly Lawn Care: +1 865-607-7520, Property Manager: 1234567890
 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2239,7 +2234,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2292,44 +2287,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="14">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2340,10 +2347,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -2381,71 +2388,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2473,7 +2480,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -2496,11 +2503,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -2509,13 +2516,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2525,7 +2532,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -2534,7 +2541,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2543,7 +2550,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2551,10 +2558,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -2619,32 +2626,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH3" zoomScale="156" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="17" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="12.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="32" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="578" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="12" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="12" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="11" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="13" width="578.005" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2744,867 +2773,867 @@
       <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
       <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="409.6000000000001">
+      <c r="A2" s="5">
         <v>1512</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>102369</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="5">
         <v>37862</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="5">
         <v>2360</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="5">
         <v>10</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="5">
         <v>3</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="5">
         <v>3</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="5">
         <v>0</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="5">
         <v>0</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="5">
-        <v>-83.608500000000006</v>
-      </c>
-      <c r="T2" s="5">
+      <c r="S2" s="7">
+        <v>-83.6085</v>
+      </c>
+      <c r="T2" s="7">
         <v>35.75112</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AB2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AD2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AF2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AG2" s="6" t="s">
         <v>56</v>
       </c>
       <c r="AH2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="409.6000000000001">
+      <c r="A3" s="5">
+        <v>1545</v>
+      </c>
+      <c r="B3" s="5">
+        <v>102402</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="5">
+        <v>37862</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="5">
+        <v>3020</v>
+      </c>
+      <c r="M3" s="5">
+        <v>15</v>
+      </c>
+      <c r="N3" s="5">
+        <v>3</v>
+      </c>
+      <c r="O3" s="5">
+        <v>3</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="7">
+        <v>-83.6179</v>
+      </c>
+      <c r="T3" s="7">
+        <v>35.71308</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI3" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="409.6000000000001">
+      <c r="A4" s="5">
+        <v>1679</v>
+      </c>
+      <c r="B4" s="5">
+        <v>102536</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="5">
+        <v>37876</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="5">
+        <v>800</v>
+      </c>
+      <c r="M4" s="5">
+        <v>6</v>
+      </c>
+      <c r="N4" s="5">
+        <v>2</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="7">
+        <v>-83.4143</v>
+      </c>
+      <c r="T4" s="7">
+        <v>35.79348</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI4" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="409.6000000000001">
+      <c r="A5" s="5">
+        <v>1849</v>
+      </c>
+      <c r="B5" s="5">
+        <v>102706</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="5">
+        <v>37862</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3000</v>
+      </c>
+      <c r="M5" s="5">
+        <v>15</v>
+      </c>
+      <c r="N5" s="5">
+        <v>5</v>
+      </c>
+      <c r="O5" s="5">
+        <v>4</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S5" s="7">
+        <v>-83.6633</v>
+      </c>
+      <c r="T5" s="7">
+        <v>35.77981</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC5" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF5" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH5" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI5" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="409.6000000000001">
+      <c r="A6" s="5">
+        <v>1899</v>
+      </c>
+      <c r="B6" s="5">
+        <v>102756</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="5">
+        <v>37862</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="5">
+        <v>1000</v>
+      </c>
+      <c r="M6" s="5">
+        <v>4</v>
+      </c>
+      <c r="N6" s="5">
+        <v>2</v>
+      </c>
+      <c r="O6" s="5">
+        <v>2</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>1</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S6" s="7">
+        <v>-83.608</v>
+      </c>
+      <c r="T6" s="7">
+        <v>35.81405</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC6" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE6" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG6" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH6" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI6" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="409.6000000000001">
+      <c r="A7" s="5">
+        <v>1900</v>
+      </c>
+      <c r="B7" s="5">
+        <v>102757</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="5">
+        <v>37862</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="5">
+        <v>2000</v>
+      </c>
+      <c r="M7" s="5">
+        <v>7</v>
+      </c>
+      <c r="N7" s="5">
+        <v>2</v>
+      </c>
+      <c r="O7" s="5">
+        <v>2</v>
+      </c>
+      <c r="P7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S7" s="7">
+        <v>-83.608</v>
+      </c>
+      <c r="T7" s="7">
+        <v>35.81405</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC7" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD7" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF7" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG7" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="AH7" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI7" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="409.6000000000001">
+      <c r="A8" s="5">
+        <v>1901</v>
+      </c>
+      <c r="B8" s="5">
+        <v>102758</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="5">
+        <v>37862</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="5">
+        <v>1000</v>
+      </c>
+      <c r="M8" s="5">
+        <v>11</v>
+      </c>
+      <c r="N8" s="5">
+        <v>4</v>
+      </c>
+      <c r="O8" s="5">
+        <v>4</v>
+      </c>
+      <c r="P8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>1</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" s="7">
+        <v>-83.608</v>
+      </c>
+      <c r="T8" s="7">
+        <v>35.81405</v>
+      </c>
+      <c r="U8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z8" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA8" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB8" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC8" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD8" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE8" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF8" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG8" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH8" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="AI8" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="1161.75">
+      <c r="A9" s="5">
+        <v>1996</v>
+      </c>
+      <c r="B9" s="5">
+        <v>102853</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" s="5">
+        <v>37876</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="5">
+        <v>2063</v>
+      </c>
+      <c r="M9" s="5">
+        <v>8</v>
+      </c>
+      <c r="N9" s="5">
+        <v>4</v>
+      </c>
+      <c r="O9" s="5">
+        <v>3</v>
+      </c>
+      <c r="P9" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="7">
+        <v>-83.5227</v>
+      </c>
+      <c r="T9" s="7">
+        <v>35.8101</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z9" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="AA9" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB9" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC9" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD9" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE9" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AF9" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="AG9" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH9" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="AI2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>1545</v>
-      </c>
-      <c r="B3" s="4">
-        <v>102402</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="4">
-        <v>37862</v>
-      </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="4">
-        <v>3020</v>
-      </c>
-      <c r="M3" s="4">
-        <v>15</v>
-      </c>
-      <c r="N3" s="4">
-        <v>3</v>
-      </c>
-      <c r="O3" s="4">
-        <v>3</v>
-      </c>
-      <c r="P3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>0</v>
-      </c>
-      <c r="R3" t="s">
-        <v>43</v>
-      </c>
-      <c r="S3" s="5">
-        <v>-83.617900000000006</v>
-      </c>
-      <c r="T3" s="5">
-        <v>35.713079999999998</v>
-      </c>
-      <c r="U3" t="s">
-        <v>44</v>
-      </c>
-      <c r="V3" t="s">
-        <v>45</v>
-      </c>
-      <c r="W3" t="s">
-        <v>46</v>
-      </c>
-      <c r="X3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>1679</v>
-      </c>
-      <c r="B4" s="4">
-        <v>102536</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="AI9" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="4">
-        <v>37876</v>
-      </c>
-      <c r="K4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" s="4">
-        <v>800</v>
-      </c>
-      <c r="M4" s="4">
-        <v>6</v>
-      </c>
-      <c r="N4" s="4">
-        <v>2</v>
-      </c>
-      <c r="O4" s="4">
-        <v>1</v>
-      </c>
-      <c r="P4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>43</v>
-      </c>
-      <c r="S4" s="5">
-        <v>-83.414299999999997</v>
-      </c>
-      <c r="T4" s="5">
-        <v>35.793480000000002</v>
-      </c>
-      <c r="U4" t="s">
-        <v>44</v>
-      </c>
-      <c r="V4" t="s">
-        <v>45</v>
-      </c>
-      <c r="W4" t="s">
-        <v>46</v>
-      </c>
-      <c r="X4" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>1849</v>
-      </c>
-      <c r="B5" s="4">
-        <v>102706</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="4">
-        <v>37862</v>
-      </c>
-      <c r="K5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="4">
-        <v>3000</v>
-      </c>
-      <c r="M5" s="4">
-        <v>15</v>
-      </c>
-      <c r="N5" s="4">
-        <v>5</v>
-      </c>
-      <c r="O5" s="4">
-        <v>4</v>
-      </c>
-      <c r="P5" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>0</v>
-      </c>
-      <c r="R5" t="s">
-        <v>43</v>
-      </c>
-      <c r="S5" s="5">
-        <v>-83.663300000000007</v>
-      </c>
-      <c r="T5" s="5">
-        <v>35.779809999999998</v>
-      </c>
-      <c r="U5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V5" t="s">
-        <v>45</v>
-      </c>
-      <c r="W5" t="s">
-        <v>46</v>
-      </c>
-      <c r="X5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>96</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>1899</v>
-      </c>
-      <c r="B6" s="4">
-        <v>102756</v>
-      </c>
-      <c r="C6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" t="s">
-        <v>107</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="4">
-        <v>37862</v>
-      </c>
-      <c r="K6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="4">
-        <v>1000</v>
-      </c>
-      <c r="M6" s="4">
-        <v>4</v>
-      </c>
-      <c r="N6" s="4">
-        <v>2</v>
-      </c>
-      <c r="O6" s="4">
-        <v>2</v>
-      </c>
-      <c r="P6" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
-        <v>43</v>
-      </c>
-      <c r="S6" s="5">
-        <v>-83.608000000000004</v>
-      </c>
-      <c r="T6" s="5">
-        <v>35.814050000000002</v>
-      </c>
-      <c r="U6" t="s">
-        <v>44</v>
-      </c>
-      <c r="V6" t="s">
-        <v>45</v>
-      </c>
-      <c r="W6" t="s">
-        <v>46</v>
-      </c>
-      <c r="X6" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>113</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>1900</v>
-      </c>
-      <c r="B7" s="4">
-        <v>102757</v>
-      </c>
-      <c r="C7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="4">
-        <v>37862</v>
-      </c>
-      <c r="K7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="4">
-        <v>2000</v>
-      </c>
-      <c r="M7" s="4">
-        <v>7</v>
-      </c>
-      <c r="N7" s="4">
-        <v>2</v>
-      </c>
-      <c r="O7" s="4">
-        <v>2</v>
-      </c>
-      <c r="P7" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>0</v>
-      </c>
-      <c r="R7" t="s">
-        <v>43</v>
-      </c>
-      <c r="S7" s="5">
-        <v>-83.608000000000004</v>
-      </c>
-      <c r="T7" s="5">
-        <v>35.814050000000002</v>
-      </c>
-      <c r="U7" t="s">
-        <v>44</v>
-      </c>
-      <c r="V7" t="s">
-        <v>45</v>
-      </c>
-      <c r="W7" t="s">
-        <v>46</v>
-      </c>
-      <c r="X7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>123</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>124</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>125</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>129</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>1901</v>
-      </c>
-      <c r="B8" s="4">
-        <v>102758</v>
-      </c>
-      <c r="C8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D8" t="s">
-        <v>133</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>134</v>
-      </c>
-      <c r="G8" t="s">
-        <v>135</v>
-      </c>
-      <c r="H8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="4">
-        <v>37862</v>
-      </c>
-      <c r="K8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="4">
-        <v>1000</v>
-      </c>
-      <c r="M8" s="4">
-        <v>11</v>
-      </c>
-      <c r="N8" s="4">
-        <v>4</v>
-      </c>
-      <c r="O8" s="4">
-        <v>4</v>
-      </c>
-      <c r="P8" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
-        <v>43</v>
-      </c>
-      <c r="S8" s="5">
-        <v>-83.608000000000004</v>
-      </c>
-      <c r="T8" s="5">
-        <v>35.814050000000002</v>
-      </c>
-      <c r="U8" t="s">
-        <v>44</v>
-      </c>
-      <c r="V8" t="s">
-        <v>45</v>
-      </c>
-      <c r="W8" t="s">
-        <v>46</v>
-      </c>
-      <c r="X8" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>136</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>137</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>138</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>139</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>141</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>143</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>144</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>145</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>1996</v>
-      </c>
-      <c r="B9" s="4">
-        <v>102853</v>
-      </c>
-      <c r="C9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G9" t="s">
-        <v>150</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="4">
-        <v>37876</v>
-      </c>
-      <c r="K9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="4">
-        <v>2063</v>
-      </c>
-      <c r="M9" s="4">
-        <v>8</v>
-      </c>
-      <c r="N9" s="4">
-        <v>4</v>
-      </c>
-      <c r="O9" s="4">
-        <v>3</v>
-      </c>
-      <c r="P9" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>0</v>
-      </c>
-      <c r="R9" t="s">
-        <v>43</v>
-      </c>
-      <c r="S9" s="5">
-        <v>-83.5227</v>
-      </c>
-      <c r="T9" s="5">
-        <v>35.810099999999998</v>
-      </c>
-      <c r="U9" t="s">
-        <v>44</v>
-      </c>
-      <c r="V9" t="s">
-        <v>45</v>
-      </c>
-      <c r="W9" t="s">
-        <v>46</v>
-      </c>
-      <c r="X9" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>151</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>152</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>153</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>154</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>155</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>156</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>158</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>159</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>160</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>